<commit_message>
Added support if wifi down, it will save till it completed
</commit_message>
<xml_diff>
--- a/src/main/resources/https___jharaphula_com_sitemap_xml.xlsx
+++ b/src/main/resources/https___jharaphula_com_sitemap_xml.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
   <si>
     <t>https://jharaphula.com/sitemap-misc.xml</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
   <si>
     <t>https://jharaphula.com/sitemap-tax-category.xml</t>
@@ -254,7 +257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -264,330 +267,528 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="F18" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="F20" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="F25" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="F38" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="F40" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="F41" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="F43" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="F46" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="F50" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="F51" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="F52" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="F53" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="F54" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="F55" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="F57" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="F58" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="F59" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="F60" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="F61" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>62</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="F63" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="F64" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="F65" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="F66" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>